<commit_message>
small change end revert to test that 0s are printed without kr
</commit_message>
<xml_diff>
--- a/test/Budget_2024.xlsx
+++ b/test/Budget_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anaki\Dokument\ANVÄNDBART\KOD\GOrdian\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409DE0C9-851C-400E-AC44-821E82A80D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D04D923-C821-41C9-B256-26ECF0F944E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14400" yWindow="0" windowWidth="14400" windowHeight="16200" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rambudget" sheetId="1" r:id="rId1"/>
@@ -3483,9 +3483,9 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5108,7 +5108,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="7"/>
-      <c r="I3" s="186"/>
+      <c r="I3" s="188"/>
       <c r="J3" s="187"/>
       <c r="K3" s="187"/>
     </row>
@@ -5129,7 +5129,7 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="7"/>
-      <c r="I4" s="186"/>
+      <c r="I4" s="188"/>
       <c r="J4" s="187"/>
       <c r="K4" s="187"/>
     </row>
@@ -5142,7 +5142,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="12"/>
-      <c r="I5" s="186"/>
+      <c r="I5" s="188"/>
       <c r="J5" s="187"/>
       <c r="K5" s="187"/>
     </row>
@@ -5157,7 +5157,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="12"/>
-      <c r="I6" s="186"/>
+      <c r="I6" s="188"/>
       <c r="J6" s="187"/>
       <c r="K6" s="187"/>
     </row>
@@ -5183,7 +5183,7 @@
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
-      <c r="I7" s="188"/>
+      <c r="I7" s="186"/>
       <c r="J7" s="187"/>
       <c r="K7" s="187"/>
     </row>
@@ -5209,7 +5209,7 @@
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
-      <c r="I8" s="188"/>
+      <c r="I8" s="186"/>
       <c r="J8" s="187"/>
       <c r="K8" s="187"/>
     </row>
@@ -5235,7 +5235,7 @@
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
-      <c r="I9" s="188"/>
+      <c r="I9" s="186"/>
       <c r="J9" s="187"/>
       <c r="K9" s="187"/>
     </row>
@@ -5261,7 +5261,7 @@
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
-      <c r="I10" s="188"/>
+      <c r="I10" s="186"/>
       <c r="J10" s="187"/>
       <c r="K10" s="187"/>
     </row>
@@ -5287,7 +5287,7 @@
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
-      <c r="I11" s="188"/>
+      <c r="I11" s="186"/>
       <c r="J11" s="187"/>
       <c r="K11" s="187"/>
     </row>
@@ -5313,7 +5313,7 @@
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
-      <c r="I12" s="188"/>
+      <c r="I12" s="186"/>
       <c r="J12" s="187"/>
       <c r="K12" s="187"/>
     </row>
@@ -5339,7 +5339,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
       <c r="H13" s="16"/>
-      <c r="I13" s="188"/>
+      <c r="I13" s="186"/>
       <c r="J13" s="187"/>
       <c r="K13" s="187"/>
     </row>
@@ -5365,7 +5365,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
       <c r="H14" s="16"/>
-      <c r="I14" s="188"/>
+      <c r="I14" s="186"/>
       <c r="J14" s="187"/>
       <c r="K14" s="187"/>
     </row>
@@ -5391,7 +5391,7 @@
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
-      <c r="I15" s="188"/>
+      <c r="I15" s="186"/>
       <c r="J15" s="187"/>
       <c r="K15" s="187"/>
     </row>
@@ -5417,7 +5417,7 @@
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
       <c r="H16" s="16"/>
-      <c r="I16" s="188"/>
+      <c r="I16" s="186"/>
       <c r="J16" s="187"/>
       <c r="K16" s="187"/>
     </row>
@@ -5443,7 +5443,7 @@
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
       <c r="H17" s="16"/>
-      <c r="I17" s="188"/>
+      <c r="I17" s="186"/>
       <c r="J17" s="187"/>
       <c r="K17" s="187"/>
     </row>
@@ -5469,7 +5469,7 @@
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
       <c r="H18" s="16"/>
-      <c r="I18" s="188"/>
+      <c r="I18" s="186"/>
       <c r="J18" s="187"/>
       <c r="K18" s="187"/>
     </row>
@@ -5495,7 +5495,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
       <c r="H19" s="16"/>
-      <c r="I19" s="188"/>
+      <c r="I19" s="186"/>
       <c r="J19" s="187"/>
       <c r="K19" s="187"/>
     </row>
@@ -5521,7 +5521,7 @@
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
-      <c r="I20" s="188"/>
+      <c r="I20" s="186"/>
       <c r="J20" s="187"/>
       <c r="K20" s="187"/>
     </row>
@@ -5547,7 +5547,7 @@
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
       <c r="H21" s="16"/>
-      <c r="I21" s="188"/>
+      <c r="I21" s="186"/>
       <c r="J21" s="187"/>
       <c r="K21" s="187"/>
     </row>
@@ -5573,7 +5573,7 @@
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
-      <c r="I22" s="188"/>
+      <c r="I22" s="186"/>
       <c r="J22" s="187"/>
       <c r="K22" s="187"/>
     </row>
@@ -5599,7 +5599,7 @@
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
       <c r="H23" s="16"/>
-      <c r="I23" s="188"/>
+      <c r="I23" s="186"/>
       <c r="J23" s="187"/>
       <c r="K23" s="187"/>
     </row>
@@ -5625,7 +5625,7 @@
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
       <c r="H24" s="16"/>
-      <c r="I24" s="188"/>
+      <c r="I24" s="186"/>
       <c r="J24" s="187"/>
       <c r="K24" s="187"/>
     </row>
@@ -5651,7 +5651,7 @@
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
       <c r="H25" s="16"/>
-      <c r="I25" s="188"/>
+      <c r="I25" s="186"/>
       <c r="J25" s="187"/>
       <c r="K25" s="187"/>
     </row>
@@ -5677,7 +5677,7 @@
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
       <c r="H26" s="16"/>
-      <c r="I26" s="188"/>
+      <c r="I26" s="186"/>
       <c r="J26" s="187"/>
       <c r="K26" s="187"/>
     </row>
@@ -5703,7 +5703,7 @@
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
       <c r="H27" s="16"/>
-      <c r="I27" s="188"/>
+      <c r="I27" s="186"/>
       <c r="J27" s="187"/>
       <c r="K27" s="187"/>
     </row>
@@ -5729,7 +5729,7 @@
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
       <c r="H28" s="16"/>
-      <c r="I28" s="188"/>
+      <c r="I28" s="186"/>
       <c r="J28" s="187"/>
       <c r="K28" s="187"/>
     </row>
@@ -5755,7 +5755,7 @@
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
       <c r="H29" s="16"/>
-      <c r="I29" s="188"/>
+      <c r="I29" s="186"/>
       <c r="J29" s="187"/>
       <c r="K29" s="187"/>
     </row>
@@ -5781,7 +5781,7 @@
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
       <c r="H30" s="16"/>
-      <c r="I30" s="188"/>
+      <c r="I30" s="186"/>
       <c r="J30" s="187"/>
       <c r="K30" s="187"/>
     </row>
@@ -5807,7 +5807,7 @@
       <c r="F31" s="16"/>
       <c r="G31" s="16"/>
       <c r="H31" s="16"/>
-      <c r="I31" s="188"/>
+      <c r="I31" s="186"/>
       <c r="J31" s="187"/>
       <c r="K31" s="187"/>
     </row>
@@ -5833,7 +5833,7 @@
       <c r="F32" s="16"/>
       <c r="G32" s="16"/>
       <c r="H32" s="16"/>
-      <c r="I32" s="188"/>
+      <c r="I32" s="186"/>
       <c r="J32" s="187"/>
       <c r="K32" s="187"/>
     </row>
@@ -5846,7 +5846,7 @@
       <c r="F33" s="16"/>
       <c r="G33" s="16"/>
       <c r="H33" s="16"/>
-      <c r="I33" s="188"/>
+      <c r="I33" s="186"/>
       <c r="J33" s="187"/>
       <c r="K33" s="187"/>
     </row>
@@ -5870,7 +5870,7 @@
       <c r="F34" s="23"/>
       <c r="G34" s="23"/>
       <c r="H34" s="23"/>
-      <c r="I34" s="188"/>
+      <c r="I34" s="186"/>
       <c r="J34" s="187"/>
       <c r="K34" s="187"/>
     </row>
@@ -5883,7 +5883,7 @@
       <c r="F35" s="23"/>
       <c r="G35" s="23"/>
       <c r="H35" s="23"/>
-      <c r="I35" s="188"/>
+      <c r="I35" s="186"/>
       <c r="J35" s="187"/>
       <c r="K35" s="187"/>
     </row>
@@ -5898,7 +5898,7 @@
       <c r="F36" s="27"/>
       <c r="G36" s="27"/>
       <c r="H36" s="27"/>
-      <c r="I36" s="186"/>
+      <c r="I36" s="188"/>
       <c r="J36" s="187"/>
       <c r="K36" s="187"/>
     </row>
@@ -5922,7 +5922,7 @@
       <c r="F37" s="27"/>
       <c r="G37" s="27"/>
       <c r="H37" s="27"/>
-      <c r="I37" s="186"/>
+      <c r="I37" s="188"/>
       <c r="J37" s="187"/>
       <c r="K37" s="187"/>
     </row>
@@ -5946,7 +5946,7 @@
       <c r="F38" s="27"/>
       <c r="G38" s="27"/>
       <c r="H38" s="27"/>
-      <c r="I38" s="186"/>
+      <c r="I38" s="188"/>
       <c r="J38" s="187"/>
       <c r="K38" s="187"/>
     </row>
@@ -5970,7 +5970,7 @@
       <c r="F39" s="27"/>
       <c r="G39" s="27"/>
       <c r="H39" s="27"/>
-      <c r="I39" s="186"/>
+      <c r="I39" s="188"/>
       <c r="J39" s="187"/>
       <c r="K39" s="187"/>
     </row>
@@ -5994,7 +5994,7 @@
       <c r="F40" s="27"/>
       <c r="G40" s="27"/>
       <c r="H40" s="27"/>
-      <c r="I40" s="186"/>
+      <c r="I40" s="188"/>
       <c r="J40" s="187"/>
       <c r="K40" s="187"/>
     </row>
@@ -6018,7 +6018,7 @@
       <c r="F41" s="27"/>
       <c r="G41" s="27"/>
       <c r="H41" s="27"/>
-      <c r="I41" s="186"/>
+      <c r="I41" s="188"/>
       <c r="J41" s="187"/>
       <c r="K41" s="187"/>
     </row>
@@ -6042,7 +6042,7 @@
       <c r="F42" s="27"/>
       <c r="G42" s="27"/>
       <c r="H42" s="27"/>
-      <c r="I42" s="186"/>
+      <c r="I42" s="188"/>
       <c r="J42" s="187"/>
       <c r="K42" s="187"/>
     </row>
@@ -6064,7 +6064,7 @@
       <c r="F43" s="27"/>
       <c r="G43" s="27"/>
       <c r="H43" s="27"/>
-      <c r="I43" s="186" t="s">
+      <c r="I43" s="188" t="s">
         <v>44</v>
       </c>
       <c r="J43" s="187"/>
@@ -6090,7 +6090,7 @@
       <c r="F44" s="27"/>
       <c r="G44" s="27"/>
       <c r="H44" s="27"/>
-      <c r="I44" s="186"/>
+      <c r="I44" s="188"/>
       <c r="J44" s="187"/>
       <c r="K44" s="187"/>
     </row>
@@ -6114,7 +6114,7 @@
       <c r="F45" s="27"/>
       <c r="G45" s="27"/>
       <c r="H45" s="27"/>
-      <c r="I45" s="186"/>
+      <c r="I45" s="188"/>
       <c r="J45" s="187"/>
       <c r="K45" s="187"/>
     </row>
@@ -6138,7 +6138,7 @@
       <c r="F46" s="27"/>
       <c r="G46" s="27"/>
       <c r="H46" s="27"/>
-      <c r="I46" s="186"/>
+      <c r="I46" s="188"/>
       <c r="J46" s="187"/>
       <c r="K46" s="187"/>
     </row>
@@ -6162,7 +6162,7 @@
       <c r="F47" s="27"/>
       <c r="G47" s="27"/>
       <c r="H47" s="27"/>
-      <c r="I47" s="186"/>
+      <c r="I47" s="188"/>
       <c r="J47" s="187"/>
       <c r="K47" s="187"/>
     </row>
@@ -6186,7 +6186,7 @@
       <c r="F48" s="27"/>
       <c r="G48" s="27"/>
       <c r="H48" s="27"/>
-      <c r="I48" s="186"/>
+      <c r="I48" s="188"/>
       <c r="J48" s="187"/>
       <c r="K48" s="187"/>
     </row>
@@ -6210,7 +6210,7 @@
       <c r="F49" s="27"/>
       <c r="G49" s="27"/>
       <c r="H49" s="27"/>
-      <c r="I49" s="186"/>
+      <c r="I49" s="188"/>
       <c r="J49" s="187"/>
       <c r="K49" s="187"/>
     </row>
@@ -6234,7 +6234,7 @@
       <c r="F50" s="27"/>
       <c r="G50" s="27"/>
       <c r="H50" s="27"/>
-      <c r="I50" s="186"/>
+      <c r="I50" s="188"/>
       <c r="J50" s="187"/>
       <c r="K50" s="187"/>
     </row>
@@ -6247,7 +6247,7 @@
       <c r="F51" s="27"/>
       <c r="G51" s="27"/>
       <c r="H51" s="27"/>
-      <c r="I51" s="186"/>
+      <c r="I51" s="188"/>
       <c r="J51" s="187"/>
       <c r="K51" s="187"/>
     </row>
@@ -6271,7 +6271,7 @@
       <c r="F52" s="27"/>
       <c r="G52" s="27"/>
       <c r="H52" s="27"/>
-      <c r="I52" s="186"/>
+      <c r="I52" s="188"/>
       <c r="J52" s="187"/>
       <c r="K52" s="187"/>
     </row>
@@ -6284,7 +6284,7 @@
       <c r="F53" s="27"/>
       <c r="G53" s="27"/>
       <c r="H53" s="27"/>
-      <c r="I53" s="186"/>
+      <c r="I53" s="188"/>
       <c r="J53" s="187"/>
       <c r="K53" s="187"/>
     </row>
@@ -6299,7 +6299,7 @@
       <c r="F54" s="27"/>
       <c r="G54" s="27"/>
       <c r="H54" s="27"/>
-      <c r="I54" s="186"/>
+      <c r="I54" s="188"/>
       <c r="J54" s="187"/>
       <c r="K54" s="187"/>
     </row>
@@ -6323,7 +6323,7 @@
       <c r="F55" s="27"/>
       <c r="G55" s="27"/>
       <c r="H55" s="27"/>
-      <c r="I55" s="186"/>
+      <c r="I55" s="188"/>
       <c r="J55" s="187"/>
       <c r="K55" s="187"/>
     </row>
@@ -6336,7 +6336,7 @@
       <c r="F56" s="27"/>
       <c r="G56" s="27"/>
       <c r="H56" s="27"/>
-      <c r="I56" s="186"/>
+      <c r="I56" s="188"/>
       <c r="J56" s="187"/>
       <c r="K56" s="187"/>
     </row>
@@ -6360,7 +6360,7 @@
       <c r="F57" s="27"/>
       <c r="G57" s="27"/>
       <c r="H57" s="27"/>
-      <c r="I57" s="186"/>
+      <c r="I57" s="188"/>
       <c r="J57" s="187"/>
       <c r="K57" s="187"/>
     </row>
@@ -6384,12 +6384,58 @@
       <c r="F58" s="27"/>
       <c r="G58" s="27"/>
       <c r="H58" s="27"/>
-      <c r="I58" s="186"/>
+      <c r="I58" s="188"/>
       <c r="J58" s="187"/>
       <c r="K58" s="187"/>
     </row>
   </sheetData>
   <mergeCells count="62">
+    <mergeCell ref="I54:K54"/>
+    <mergeCell ref="I55:K55"/>
+    <mergeCell ref="I56:K56"/>
+    <mergeCell ref="I57:K57"/>
+    <mergeCell ref="I58:K58"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="I41:K41"/>
+    <mergeCell ref="I42:K42"/>
+    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="I40:K40"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="I36:K36"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I46:K46"/>
+    <mergeCell ref="I47:K47"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I39:K39"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:G2"/>
     <mergeCell ref="I11:K11"/>
     <mergeCell ref="I12:K12"/>
     <mergeCell ref="I51:K51"/>
@@ -6401,57 +6447,11 @@
     <mergeCell ref="I26:K26"/>
     <mergeCell ref="I44:K44"/>
     <mergeCell ref="I45:K45"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I46:K46"/>
-    <mergeCell ref="I47:K47"/>
     <mergeCell ref="I49:K49"/>
     <mergeCell ref="I50:K50"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I22:K22"/>
     <mergeCell ref="I48:K48"/>
-    <mergeCell ref="I39:K39"/>
     <mergeCell ref="I37:K37"/>
     <mergeCell ref="I38:K38"/>
-    <mergeCell ref="I41:K41"/>
-    <mergeCell ref="I42:K42"/>
-    <mergeCell ref="I43:K43"/>
-    <mergeCell ref="I40:K40"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="I36:K36"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="I54:K54"/>
-    <mergeCell ref="I55:K55"/>
-    <mergeCell ref="I56:K56"/>
-    <mergeCell ref="I57:K57"/>
-    <mergeCell ref="I58:K58"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:K58">
     <cfRule type="cellIs" dxfId="155" priority="1" operator="greaterThan">
@@ -9038,7 +9038,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="13.2">
       <c r="A2" s="143" t="s">
         <v>630</v>
       </c>
@@ -9050,7 +9050,7 @@
       <c r="G2" s="154"/>
       <c r="H2" s="154"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" ht="13.2">
       <c r="A3" s="152"/>
       <c r="B3" s="143" t="s">
         <v>61</v>
@@ -9062,7 +9062,7 @@
       <c r="G3" s="154"/>
       <c r="H3" s="154"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" ht="13.2">
       <c r="A4" s="152"/>
       <c r="B4" s="143"/>
       <c r="C4" s="152" t="s">
@@ -9077,7 +9077,7 @@
       <c r="G4" s="154"/>
       <c r="H4" s="154"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" ht="13.2">
       <c r="A5" s="152"/>
       <c r="B5" s="143"/>
       <c r="C5" s="152" t="s">
@@ -9094,7 +9094,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" ht="13.2">
       <c r="A6" s="152"/>
       <c r="B6" s="143"/>
       <c r="C6" s="152" t="s">
@@ -9111,7 +9111,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" ht="13.2">
       <c r="A7" s="152"/>
       <c r="B7" s="143"/>
       <c r="C7" s="152"/>
@@ -9120,7 +9120,7 @@
       <c r="G7" s="154"/>
       <c r="H7" s="154"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="13.2">
       <c r="A8" s="152"/>
       <c r="B8" s="143"/>
       <c r="C8" s="143" t="s">
@@ -9137,7 +9137,7 @@
       <c r="G8" s="157"/>
       <c r="H8" s="157"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" ht="13.2">
       <c r="A9" s="152"/>
       <c r="B9" s="143"/>
       <c r="C9" s="143"/>
@@ -9146,7 +9146,7 @@
       <c r="G9" s="157"/>
       <c r="H9" s="157"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" ht="13.2">
       <c r="A10" s="152"/>
       <c r="B10" s="143"/>
       <c r="C10" s="143" t="s">
@@ -9163,7 +9163,7 @@
       <c r="G10" s="157"/>
       <c r="H10" s="157"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" ht="13.2">
       <c r="A11" s="152"/>
       <c r="B11" s="152"/>
       <c r="C11" s="152"/>
@@ -9260,7 +9260,7 @@
       <c r="G2" s="35"/>
       <c r="H2" s="159"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" ht="13.2">
       <c r="A3" s="34"/>
       <c r="B3" s="89" t="s">
         <v>61</v>
@@ -9346,7 +9346,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="13.2">
       <c r="A8" s="34"/>
       <c r="B8" s="89"/>
       <c r="C8" s="34"/>
@@ -9377,7 +9377,7 @@
       </c>
       <c r="H9" s="159"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" ht="13.2">
       <c r="A10" s="34"/>
       <c r="B10" s="34"/>
       <c r="C10" s="34"/>
@@ -9408,7 +9408,7 @@
       </c>
       <c r="H11" s="76"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" ht="13.2">
       <c r="A12" s="34"/>
       <c r="B12" s="34"/>
       <c r="C12" s="34"/>
@@ -9507,7 +9507,7 @@
       <c r="G2" s="35"/>
       <c r="H2" s="35"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" ht="13.2">
       <c r="A3" s="34"/>
       <c r="B3" s="89" t="s">
         <v>61</v>
@@ -9573,7 +9573,7 @@
       <c r="G6" s="35"/>
       <c r="H6" s="35"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" ht="13.2">
       <c r="A7" s="34"/>
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
@@ -9629,7 +9629,7 @@
       <c r="G10" s="35"/>
       <c r="H10" s="35"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" ht="13.2">
       <c r="A11" s="34"/>
       <c r="B11" s="34"/>
       <c r="C11" s="34"/>
@@ -10198,7 +10198,7 @@
       <c r="G2" s="35"/>
       <c r="H2" s="35"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" ht="13.2">
       <c r="A3" s="34"/>
       <c r="B3" s="89" t="s">
         <v>61</v>
@@ -10340,7 +10340,7 @@
       <c r="G11" s="35"/>
       <c r="H11" s="35"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" ht="13.2">
       <c r="A12" s="34"/>
       <c r="B12" s="34"/>
       <c r="C12" s="34"/>
@@ -10434,7 +10434,7 @@
       <c r="G18" s="35"/>
       <c r="H18" s="35"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" ht="13.2">
       <c r="A19" s="34"/>
       <c r="B19" s="34"/>
       <c r="G19" s="35"/>
@@ -11193,9 +11193,9 @@
   </sheetPr>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -14050,7 +14050,7 @@
       <c r="G2" s="35"/>
       <c r="H2" s="35"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" ht="13.2">
       <c r="A3" s="34"/>
       <c r="B3" s="89" t="s">
         <v>61</v>
@@ -14147,7 +14147,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" ht="13.2">
       <c r="A9" s="34"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
@@ -15692,7 +15692,7 @@
       <c r="G5" s="36"/>
       <c r="H5" s="36"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" ht="13.2">
       <c r="A6" s="34"/>
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
@@ -15718,7 +15718,7 @@
       <c r="G7" s="36"/>
       <c r="H7" s="36"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="13.2">
       <c r="A8" s="34"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
@@ -15744,7 +15744,7 @@
       <c r="G9" s="78"/>
       <c r="H9" s="78"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" ht="13.2">
       <c r="A10" s="34"/>
       <c r="B10" s="34"/>
       <c r="C10" s="34"/>
@@ -22164,7 +22164,7 @@
       <c r="G4" s="36"/>
       <c r="H4" s="149"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" ht="16.2">
       <c r="A5" s="34"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
@@ -22189,7 +22189,7 @@
       <c r="G6" s="36"/>
       <c r="H6" s="149"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" ht="16.2">
       <c r="A7" s="34"/>
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
@@ -22281,7 +22281,7 @@
       <c r="G13" s="36"/>
       <c r="H13" s="149"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" ht="16.2">
       <c r="A14" s="34"/>
       <c r="B14" s="34"/>
       <c r="C14" s="34"/>
@@ -22306,7 +22306,7 @@
       <c r="G15" s="36"/>
       <c r="H15" s="149"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" ht="16.2">
       <c r="A16" s="34"/>
       <c r="B16" s="34"/>
       <c r="C16" s="34"/>
@@ -22331,7 +22331,7 @@
       <c r="G17" s="36"/>
       <c r="H17" s="149"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" ht="16.2">
       <c r="A18" s="34"/>
       <c r="B18" s="34"/>
       <c r="C18" s="34"/>
@@ -22397,7 +22397,7 @@
       <c r="G22" s="36"/>
       <c r="H22" s="149"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" ht="16.2">
       <c r="A23" s="34"/>
       <c r="B23" s="34"/>
       <c r="C23" s="34"/>
@@ -23077,7 +23077,7 @@
       <c r="G7" s="149"/>
       <c r="H7" s="149"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="16.2">
       <c r="A8" s="34"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
@@ -23374,7 +23374,7 @@
   </sheetPr>
   <dimension ref="A1:H161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
@@ -27493,7 +27493,7 @@
       <c r="G2" s="35"/>
       <c r="H2" s="76"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" ht="13.2">
       <c r="A3" s="34"/>
       <c r="B3" s="34" t="s">
         <v>61</v>
@@ -27635,7 +27635,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" ht="13.2">
       <c r="A11" s="34"/>
       <c r="B11" s="34"/>
       <c r="C11" s="34"/>
@@ -27666,7 +27666,7 @@
       </c>
       <c r="H12" s="76"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" ht="13.2">
       <c r="A13" s="34"/>
       <c r="B13" s="34"/>
       <c r="C13" s="34"/>
@@ -27697,7 +27697,7 @@
       </c>
       <c r="H14" s="76"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" ht="13.2">
       <c r="A15" s="34"/>
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
@@ -28122,7 +28122,7 @@
       <c r="G23" s="78"/>
       <c r="H23" s="77"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" ht="13.2">
       <c r="A24" s="34"/>
       <c r="B24" s="34"/>
       <c r="C24" s="34"/>
@@ -30341,7 +30341,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="13.2">
       <c r="A2" s="89" t="s">
         <v>16</v>
       </c>
@@ -30353,7 +30353,7 @@
       <c r="G2" s="78"/>
       <c r="H2" s="78"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" ht="13.2">
       <c r="A3" s="34"/>
       <c r="B3" s="91" t="s">
         <v>370</v>
@@ -30365,7 +30365,7 @@
       <c r="G3" s="78"/>
       <c r="H3" s="78"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" ht="13.2">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34" t="s">
@@ -30381,7 +30381,7 @@
       <c r="G4" s="78"/>
       <c r="H4" s="78"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" ht="13.2">
       <c r="A5" s="34"/>
       <c r="B5" s="94"/>
       <c r="C5" s="94" t="s">
@@ -30397,7 +30397,7 @@
       <c r="G5" s="95"/>
       <c r="H5" s="95"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" ht="13.2">
       <c r="A6" s="34"/>
       <c r="B6" s="34"/>
       <c r="C6" s="34" t="s">
@@ -30413,7 +30413,7 @@
       <c r="G6" s="78"/>
       <c r="H6" s="78"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" ht="13.2">
       <c r="A7" s="34"/>
       <c r="B7" s="34"/>
       <c r="C7" s="34" t="s">
@@ -30429,7 +30429,7 @@
       <c r="G7" s="78"/>
       <c r="H7" s="78"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="13.2">
       <c r="A8" s="34"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34" t="s">
@@ -30445,7 +30445,7 @@
       <c r="G8" s="78"/>
       <c r="H8" s="78"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" ht="13.2">
       <c r="A9" s="34"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34" t="s">
@@ -30461,7 +30461,7 @@
       <c r="G9" s="78"/>
       <c r="H9" s="78"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" ht="13.2">
       <c r="A10" s="34"/>
       <c r="B10" s="34"/>
       <c r="C10" s="34"/>
@@ -30471,7 +30471,7 @@
       <c r="G10" s="78"/>
       <c r="H10" s="78"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" ht="13.2">
       <c r="A11" s="34"/>
       <c r="B11" s="34"/>
       <c r="C11" s="89" t="s">
@@ -30489,7 +30489,7 @@
       <c r="G11" s="78"/>
       <c r="H11" s="78"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" ht="13.2">
       <c r="A12" s="34"/>
       <c r="B12" s="34"/>
       <c r="C12" s="34"/>
@@ -30499,7 +30499,7 @@
       <c r="G12" s="78"/>
       <c r="H12" s="78"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" ht="13.2">
       <c r="A13" s="34"/>
       <c r="B13" s="98" t="s">
         <v>374</v>
@@ -30511,7 +30511,7 @@
       <c r="G13" s="95"/>
       <c r="H13" s="95"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" ht="13.2">
       <c r="A14" s="34"/>
       <c r="B14" s="94"/>
       <c r="C14" s="94" t="s">
@@ -30527,7 +30527,7 @@
       <c r="G14" s="95"/>
       <c r="H14" s="95"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" ht="13.2">
       <c r="A15" s="34"/>
       <c r="B15" s="94"/>
       <c r="C15" s="94" t="s">
@@ -30543,7 +30543,7 @@
       <c r="G15" s="95"/>
       <c r="H15" s="95"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" ht="13.2">
       <c r="A16" s="34"/>
       <c r="B16" s="94"/>
       <c r="C16" s="94"/>
@@ -30553,7 +30553,7 @@
       <c r="G16" s="95"/>
       <c r="H16" s="95"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" ht="13.2">
       <c r="A17" s="34"/>
       <c r="B17" s="94"/>
       <c r="C17" s="98" t="s">
@@ -30569,7 +30569,7 @@
       <c r="G17" s="95"/>
       <c r="H17" s="95"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" ht="13.2">
       <c r="A18" s="34"/>
       <c r="B18" s="89"/>
       <c r="C18" s="34"/>
@@ -30579,7 +30579,7 @@
       <c r="G18" s="78"/>
       <c r="H18" s="78"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" ht="13.2">
       <c r="A19" s="34"/>
       <c r="B19" s="100" t="s">
         <v>375</v>
@@ -30591,7 +30591,7 @@
       <c r="G19" s="78"/>
       <c r="H19" s="78"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" ht="13.2">
       <c r="A20" s="34"/>
       <c r="B20" s="94"/>
       <c r="C20" s="94" t="s">
@@ -30607,7 +30607,7 @@
       <c r="G20" s="95"/>
       <c r="H20" s="95"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" ht="13.2">
       <c r="A21" s="34"/>
       <c r="B21" s="34"/>
       <c r="C21" s="34" t="s">
@@ -30623,7 +30623,7 @@
       <c r="G21" s="78"/>
       <c r="H21" s="78"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" ht="13.2">
       <c r="A22" s="34"/>
       <c r="B22" s="34"/>
       <c r="C22" s="34"/>
@@ -30633,7 +30633,7 @@
       <c r="G22" s="78"/>
       <c r="H22" s="78"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" ht="13.2">
       <c r="A23" s="34"/>
       <c r="B23" s="34"/>
       <c r="C23" s="89" t="s">
@@ -30649,7 +30649,7 @@
       <c r="G23" s="78"/>
       <c r="H23" s="78"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" ht="13.2">
       <c r="A24" s="34"/>
       <c r="B24" s="34"/>
       <c r="C24" s="34"/>

</xml_diff>

<commit_message>
scary update to budget file
</commit_message>
<xml_diff>
--- a/test/Budget_2024.xlsx
+++ b/test/Budget_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anaki\Dokument\ANVÄNDBART\KOD\GOrdian\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D04D923-C821-41C9-B256-26ECF0F944E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4ADCE3A-E5A6-455A-8517-FE8078CAEB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rambudget" sheetId="1" r:id="rId1"/>
@@ -3483,9 +3483,9 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5108,7 +5108,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="7"/>
-      <c r="I3" s="188"/>
+      <c r="I3" s="186"/>
       <c r="J3" s="187"/>
       <c r="K3" s="187"/>
     </row>
@@ -5129,7 +5129,7 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="7"/>
-      <c r="I4" s="188"/>
+      <c r="I4" s="186"/>
       <c r="J4" s="187"/>
       <c r="K4" s="187"/>
     </row>
@@ -5142,7 +5142,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="12"/>
-      <c r="I5" s="188"/>
+      <c r="I5" s="186"/>
       <c r="J5" s="187"/>
       <c r="K5" s="187"/>
     </row>
@@ -5157,7 +5157,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="12"/>
-      <c r="I6" s="188"/>
+      <c r="I6" s="186"/>
       <c r="J6" s="187"/>
       <c r="K6" s="187"/>
     </row>
@@ -5183,7 +5183,7 @@
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
-      <c r="I7" s="186"/>
+      <c r="I7" s="188"/>
       <c r="J7" s="187"/>
       <c r="K7" s="187"/>
     </row>
@@ -5209,7 +5209,7 @@
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
-      <c r="I8" s="186"/>
+      <c r="I8" s="188"/>
       <c r="J8" s="187"/>
       <c r="K8" s="187"/>
     </row>
@@ -5235,7 +5235,7 @@
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
-      <c r="I9" s="186"/>
+      <c r="I9" s="188"/>
       <c r="J9" s="187"/>
       <c r="K9" s="187"/>
     </row>
@@ -5261,7 +5261,7 @@
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
-      <c r="I10" s="186"/>
+      <c r="I10" s="188"/>
       <c r="J10" s="187"/>
       <c r="K10" s="187"/>
     </row>
@@ -5287,7 +5287,7 @@
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
-      <c r="I11" s="186"/>
+      <c r="I11" s="188"/>
       <c r="J11" s="187"/>
       <c r="K11" s="187"/>
     </row>
@@ -5313,7 +5313,7 @@
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
-      <c r="I12" s="186"/>
+      <c r="I12" s="188"/>
       <c r="J12" s="187"/>
       <c r="K12" s="187"/>
     </row>
@@ -5339,7 +5339,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
       <c r="H13" s="16"/>
-      <c r="I13" s="186"/>
+      <c r="I13" s="188"/>
       <c r="J13" s="187"/>
       <c r="K13" s="187"/>
     </row>
@@ -5365,7 +5365,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
       <c r="H14" s="16"/>
-      <c r="I14" s="186"/>
+      <c r="I14" s="188"/>
       <c r="J14" s="187"/>
       <c r="K14" s="187"/>
     </row>
@@ -5391,7 +5391,7 @@
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
-      <c r="I15" s="186"/>
+      <c r="I15" s="188"/>
       <c r="J15" s="187"/>
       <c r="K15" s="187"/>
     </row>
@@ -5417,7 +5417,7 @@
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
       <c r="H16" s="16"/>
-      <c r="I16" s="186"/>
+      <c r="I16" s="188"/>
       <c r="J16" s="187"/>
       <c r="K16" s="187"/>
     </row>
@@ -5443,7 +5443,7 @@
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
       <c r="H17" s="16"/>
-      <c r="I17" s="186"/>
+      <c r="I17" s="188"/>
       <c r="J17" s="187"/>
       <c r="K17" s="187"/>
     </row>
@@ -5469,7 +5469,7 @@
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
       <c r="H18" s="16"/>
-      <c r="I18" s="186"/>
+      <c r="I18" s="188"/>
       <c r="J18" s="187"/>
       <c r="K18" s="187"/>
     </row>
@@ -5495,7 +5495,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
       <c r="H19" s="16"/>
-      <c r="I19" s="186"/>
+      <c r="I19" s="188"/>
       <c r="J19" s="187"/>
       <c r="K19" s="187"/>
     </row>
@@ -5521,7 +5521,7 @@
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
-      <c r="I20" s="186"/>
+      <c r="I20" s="188"/>
       <c r="J20" s="187"/>
       <c r="K20" s="187"/>
     </row>
@@ -5547,7 +5547,7 @@
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
       <c r="H21" s="16"/>
-      <c r="I21" s="186"/>
+      <c r="I21" s="188"/>
       <c r="J21" s="187"/>
       <c r="K21" s="187"/>
     </row>
@@ -5573,7 +5573,7 @@
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
-      <c r="I22" s="186"/>
+      <c r="I22" s="188"/>
       <c r="J22" s="187"/>
       <c r="K22" s="187"/>
     </row>
@@ -5599,7 +5599,7 @@
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
       <c r="H23" s="16"/>
-      <c r="I23" s="186"/>
+      <c r="I23" s="188"/>
       <c r="J23" s="187"/>
       <c r="K23" s="187"/>
     </row>
@@ -5625,7 +5625,7 @@
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
       <c r="H24" s="16"/>
-      <c r="I24" s="186"/>
+      <c r="I24" s="188"/>
       <c r="J24" s="187"/>
       <c r="K24" s="187"/>
     </row>
@@ -5651,7 +5651,7 @@
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
       <c r="H25" s="16"/>
-      <c r="I25" s="186"/>
+      <c r="I25" s="188"/>
       <c r="J25" s="187"/>
       <c r="K25" s="187"/>
     </row>
@@ -5677,7 +5677,7 @@
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
       <c r="H26" s="16"/>
-      <c r="I26" s="186"/>
+      <c r="I26" s="188"/>
       <c r="J26" s="187"/>
       <c r="K26" s="187"/>
     </row>
@@ -5703,7 +5703,7 @@
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
       <c r="H27" s="16"/>
-      <c r="I27" s="186"/>
+      <c r="I27" s="188"/>
       <c r="J27" s="187"/>
       <c r="K27" s="187"/>
     </row>
@@ -5729,7 +5729,7 @@
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
       <c r="H28" s="16"/>
-      <c r="I28" s="186"/>
+      <c r="I28" s="188"/>
       <c r="J28" s="187"/>
       <c r="K28" s="187"/>
     </row>
@@ -5755,7 +5755,7 @@
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
       <c r="H29" s="16"/>
-      <c r="I29" s="186"/>
+      <c r="I29" s="188"/>
       <c r="J29" s="187"/>
       <c r="K29" s="187"/>
     </row>
@@ -5781,7 +5781,7 @@
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
       <c r="H30" s="16"/>
-      <c r="I30" s="186"/>
+      <c r="I30" s="188"/>
       <c r="J30" s="187"/>
       <c r="K30" s="187"/>
     </row>
@@ -5807,7 +5807,7 @@
       <c r="F31" s="16"/>
       <c r="G31" s="16"/>
       <c r="H31" s="16"/>
-      <c r="I31" s="186"/>
+      <c r="I31" s="188"/>
       <c r="J31" s="187"/>
       <c r="K31" s="187"/>
     </row>
@@ -5833,7 +5833,7 @@
       <c r="F32" s="16"/>
       <c r="G32" s="16"/>
       <c r="H32" s="16"/>
-      <c r="I32" s="186"/>
+      <c r="I32" s="188"/>
       <c r="J32" s="187"/>
       <c r="K32" s="187"/>
     </row>
@@ -5846,7 +5846,7 @@
       <c r="F33" s="16"/>
       <c r="G33" s="16"/>
       <c r="H33" s="16"/>
-      <c r="I33" s="186"/>
+      <c r="I33" s="188"/>
       <c r="J33" s="187"/>
       <c r="K33" s="187"/>
     </row>
@@ -5870,7 +5870,7 @@
       <c r="F34" s="23"/>
       <c r="G34" s="23"/>
       <c r="H34" s="23"/>
-      <c r="I34" s="186"/>
+      <c r="I34" s="188"/>
       <c r="J34" s="187"/>
       <c r="K34" s="187"/>
     </row>
@@ -5883,7 +5883,7 @@
       <c r="F35" s="23"/>
       <c r="G35" s="23"/>
       <c r="H35" s="23"/>
-      <c r="I35" s="186"/>
+      <c r="I35" s="188"/>
       <c r="J35" s="187"/>
       <c r="K35" s="187"/>
     </row>
@@ -5898,7 +5898,7 @@
       <c r="F36" s="27"/>
       <c r="G36" s="27"/>
       <c r="H36" s="27"/>
-      <c r="I36" s="188"/>
+      <c r="I36" s="186"/>
       <c r="J36" s="187"/>
       <c r="K36" s="187"/>
     </row>
@@ -5922,7 +5922,7 @@
       <c r="F37" s="27"/>
       <c r="G37" s="27"/>
       <c r="H37" s="27"/>
-      <c r="I37" s="188"/>
+      <c r="I37" s="186"/>
       <c r="J37" s="187"/>
       <c r="K37" s="187"/>
     </row>
@@ -5946,7 +5946,7 @@
       <c r="F38" s="27"/>
       <c r="G38" s="27"/>
       <c r="H38" s="27"/>
-      <c r="I38" s="188"/>
+      <c r="I38" s="186"/>
       <c r="J38" s="187"/>
       <c r="K38" s="187"/>
     </row>
@@ -5970,7 +5970,7 @@
       <c r="F39" s="27"/>
       <c r="G39" s="27"/>
       <c r="H39" s="27"/>
-      <c r="I39" s="188"/>
+      <c r="I39" s="186"/>
       <c r="J39" s="187"/>
       <c r="K39" s="187"/>
     </row>
@@ -5994,7 +5994,7 @@
       <c r="F40" s="27"/>
       <c r="G40" s="27"/>
       <c r="H40" s="27"/>
-      <c r="I40" s="188"/>
+      <c r="I40" s="186"/>
       <c r="J40" s="187"/>
       <c r="K40" s="187"/>
     </row>
@@ -6018,7 +6018,7 @@
       <c r="F41" s="27"/>
       <c r="G41" s="27"/>
       <c r="H41" s="27"/>
-      <c r="I41" s="188"/>
+      <c r="I41" s="186"/>
       <c r="J41" s="187"/>
       <c r="K41" s="187"/>
     </row>
@@ -6042,7 +6042,7 @@
       <c r="F42" s="27"/>
       <c r="G42" s="27"/>
       <c r="H42" s="27"/>
-      <c r="I42" s="188"/>
+      <c r="I42" s="186"/>
       <c r="J42" s="187"/>
       <c r="K42" s="187"/>
     </row>
@@ -6064,7 +6064,7 @@
       <c r="F43" s="27"/>
       <c r="G43" s="27"/>
       <c r="H43" s="27"/>
-      <c r="I43" s="188" t="s">
+      <c r="I43" s="186" t="s">
         <v>44</v>
       </c>
       <c r="J43" s="187"/>
@@ -6090,7 +6090,7 @@
       <c r="F44" s="27"/>
       <c r="G44" s="27"/>
       <c r="H44" s="27"/>
-      <c r="I44" s="188"/>
+      <c r="I44" s="186"/>
       <c r="J44" s="187"/>
       <c r="K44" s="187"/>
     </row>
@@ -6114,7 +6114,7 @@
       <c r="F45" s="27"/>
       <c r="G45" s="27"/>
       <c r="H45" s="27"/>
-      <c r="I45" s="188"/>
+      <c r="I45" s="186"/>
       <c r="J45" s="187"/>
       <c r="K45" s="187"/>
     </row>
@@ -6138,7 +6138,7 @@
       <c r="F46" s="27"/>
       <c r="G46" s="27"/>
       <c r="H46" s="27"/>
-      <c r="I46" s="188"/>
+      <c r="I46" s="186"/>
       <c r="J46" s="187"/>
       <c r="K46" s="187"/>
     </row>
@@ -6162,7 +6162,7 @@
       <c r="F47" s="27"/>
       <c r="G47" s="27"/>
       <c r="H47" s="27"/>
-      <c r="I47" s="188"/>
+      <c r="I47" s="186"/>
       <c r="J47" s="187"/>
       <c r="K47" s="187"/>
     </row>
@@ -6186,7 +6186,7 @@
       <c r="F48" s="27"/>
       <c r="G48" s="27"/>
       <c r="H48" s="27"/>
-      <c r="I48" s="188"/>
+      <c r="I48" s="186"/>
       <c r="J48" s="187"/>
       <c r="K48" s="187"/>
     </row>
@@ -6210,7 +6210,7 @@
       <c r="F49" s="27"/>
       <c r="G49" s="27"/>
       <c r="H49" s="27"/>
-      <c r="I49" s="188"/>
+      <c r="I49" s="186"/>
       <c r="J49" s="187"/>
       <c r="K49" s="187"/>
     </row>
@@ -6234,7 +6234,7 @@
       <c r="F50" s="27"/>
       <c r="G50" s="27"/>
       <c r="H50" s="27"/>
-      <c r="I50" s="188"/>
+      <c r="I50" s="186"/>
       <c r="J50" s="187"/>
       <c r="K50" s="187"/>
     </row>
@@ -6247,7 +6247,7 @@
       <c r="F51" s="27"/>
       <c r="G51" s="27"/>
       <c r="H51" s="27"/>
-      <c r="I51" s="188"/>
+      <c r="I51" s="186"/>
       <c r="J51" s="187"/>
       <c r="K51" s="187"/>
     </row>
@@ -6271,7 +6271,7 @@
       <c r="F52" s="27"/>
       <c r="G52" s="27"/>
       <c r="H52" s="27"/>
-      <c r="I52" s="188"/>
+      <c r="I52" s="186"/>
       <c r="J52" s="187"/>
       <c r="K52" s="187"/>
     </row>
@@ -6284,7 +6284,7 @@
       <c r="F53" s="27"/>
       <c r="G53" s="27"/>
       <c r="H53" s="27"/>
-      <c r="I53" s="188"/>
+      <c r="I53" s="186"/>
       <c r="J53" s="187"/>
       <c r="K53" s="187"/>
     </row>
@@ -6299,7 +6299,7 @@
       <c r="F54" s="27"/>
       <c r="G54" s="27"/>
       <c r="H54" s="27"/>
-      <c r="I54" s="188"/>
+      <c r="I54" s="186"/>
       <c r="J54" s="187"/>
       <c r="K54" s="187"/>
     </row>
@@ -6323,7 +6323,7 @@
       <c r="F55" s="27"/>
       <c r="G55" s="27"/>
       <c r="H55" s="27"/>
-      <c r="I55" s="188"/>
+      <c r="I55" s="186"/>
       <c r="J55" s="187"/>
       <c r="K55" s="187"/>
     </row>
@@ -6336,7 +6336,7 @@
       <c r="F56" s="27"/>
       <c r="G56" s="27"/>
       <c r="H56" s="27"/>
-      <c r="I56" s="188"/>
+      <c r="I56" s="186"/>
       <c r="J56" s="187"/>
       <c r="K56" s="187"/>
     </row>
@@ -6360,7 +6360,7 @@
       <c r="F57" s="27"/>
       <c r="G57" s="27"/>
       <c r="H57" s="27"/>
-      <c r="I57" s="188"/>
+      <c r="I57" s="186"/>
       <c r="J57" s="187"/>
       <c r="K57" s="187"/>
     </row>
@@ -6384,31 +6384,39 @@
       <c r="F58" s="27"/>
       <c r="G58" s="27"/>
       <c r="H58" s="27"/>
-      <c r="I58" s="188"/>
+      <c r="I58" s="186"/>
       <c r="J58" s="187"/>
       <c r="K58" s="187"/>
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="I54:K54"/>
-    <mergeCell ref="I55:K55"/>
-    <mergeCell ref="I56:K56"/>
-    <mergeCell ref="I57:K57"/>
-    <mergeCell ref="I58:K58"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="I41:K41"/>
-    <mergeCell ref="I42:K42"/>
-    <mergeCell ref="I43:K43"/>
-    <mergeCell ref="I40:K40"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="I36:K36"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="I51:K51"/>
+    <mergeCell ref="I52:K52"/>
+    <mergeCell ref="I53:K53"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="I44:K44"/>
+    <mergeCell ref="I45:K45"/>
+    <mergeCell ref="I49:K49"/>
+    <mergeCell ref="I50:K50"/>
+    <mergeCell ref="I48:K48"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="I38:K38"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I7:K7"/>
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="I10:K10"/>
@@ -6425,33 +6433,25 @@
     <mergeCell ref="I21:K21"/>
     <mergeCell ref="I22:K22"/>
     <mergeCell ref="I39:K39"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="I51:K51"/>
-    <mergeCell ref="I52:K52"/>
-    <mergeCell ref="I53:K53"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="I44:K44"/>
-    <mergeCell ref="I45:K45"/>
-    <mergeCell ref="I49:K49"/>
-    <mergeCell ref="I50:K50"/>
-    <mergeCell ref="I48:K48"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="I38:K38"/>
+    <mergeCell ref="I41:K41"/>
+    <mergeCell ref="I42:K42"/>
+    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="I40:K40"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="I36:K36"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="I54:K54"/>
+    <mergeCell ref="I55:K55"/>
+    <mergeCell ref="I56:K56"/>
+    <mergeCell ref="I57:K57"/>
+    <mergeCell ref="I58:K58"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:K58">
     <cfRule type="cellIs" dxfId="155" priority="1" operator="greaterThan">
@@ -11195,7 +11195,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -11941,6 +11941,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added types to some budget sheets
</commit_message>
<xml_diff>
--- a/test/Budget_2024.xlsx
+++ b/test/Budget_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anaki\Dokument\ANVÄNDBART\KOD\GOrdian\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4ADCE3A-E5A6-455A-8517-FE8078CAEB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176B2E8D-A92B-473A-A7C5-00CC8584FDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rambudget" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2345" uniqueCount="895">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2349" uniqueCount="897">
   <si>
     <t>Konglig Datasektionen Budget 2024</t>
   </si>
@@ -2758,6 +2758,12 @@
   </si>
   <si>
     <t>Inspelningskostnader</t>
+  </si>
+  <si>
+    <t>Nämnd</t>
+  </si>
+  <si>
+    <t>Övrigt</t>
   </si>
 </sst>
 </file>
@@ -2771,7 +2777,7 @@
     <numFmt numFmtId="167" formatCode="#,##0.00[$kr]"/>
     <numFmt numFmtId="168" formatCode="#,##0&quot;kr&quot;"/>
   </numFmts>
-  <fonts count="43">
+  <fonts count="46">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3009,6 +3015,25 @@
       <color rgb="FF000000"/>
       <name val="Lato"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Lato"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Lato"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -3108,7 +3133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="194">
+  <cellXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3497,6 +3522,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11193,9 +11221,9 @@
   </sheetPr>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -11246,7 +11274,9 @@
       <c r="H2" s="36"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A3" s="34"/>
+      <c r="A3" s="196" t="s">
+        <v>896</v>
+      </c>
       <c r="B3" s="33" t="s">
         <v>61</v>
       </c>
@@ -15785,9 +15815,9 @@
   </sheetPr>
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -15838,7 +15868,9 @@
       <c r="H2" s="52"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A3" s="8"/>
+      <c r="A3" s="194" t="s">
+        <v>895</v>
+      </c>
       <c r="B3" s="49" t="s">
         <v>61</v>
       </c>
@@ -22089,7 +22121,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -23377,7 +23409,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -23428,7 +23460,9 @@
       <c r="H2" s="65"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A3" s="1"/>
+      <c r="A3" s="194" t="s">
+        <v>36</v>
+      </c>
       <c r="B3" s="33" t="s">
         <v>61</v>
       </c>
@@ -26118,8 +26152,8 @@
   <dimension ref="A1:H72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -27168,7 +27202,7 @@
     <row r="69" spans="1:8" ht="16.2">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
-      <c r="C69" s="33" t="s">
+      <c r="C69" s="195" t="s">
         <v>111</v>
       </c>
       <c r="D69" s="68"/>
@@ -27254,7 +27288,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -27444,7 +27478,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -27495,7 +27529,9 @@
       <c r="H2" s="76"/>
     </row>
     <row r="3" spans="1:8" ht="13.2">
-      <c r="A3" s="34"/>
+      <c r="A3" s="196" t="s">
+        <v>895</v>
+      </c>
       <c r="B3" s="34" t="s">
         <v>61</v>
       </c>

</xml_diff>